<commit_message>
Identificacao dos casos de uso
</commit_message>
<xml_diff>
--- a/Requisitos e Casos de Uso.xlsx
+++ b/Requisitos e Casos de Uso.xlsx
@@ -1,22 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="23416"/>
+  <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="12240" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="100" windowWidth="12240" windowHeight="8020"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
     <sheet name="Plan2" sheetId="2" r:id="rId2"/>
     <sheet name="Plan3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="77">
   <si>
     <t>REQUISITOS DO SISTEMA</t>
   </si>
@@ -168,13 +173,94 @@
   </si>
   <si>
     <t>Autenticar usuário                                             Gerenciar permissões</t>
+  </si>
+  <si>
+    <t>ATOR(ES)</t>
+  </si>
+  <si>
+    <t>UC01</t>
+  </si>
+  <si>
+    <t>UC02</t>
+  </si>
+  <si>
+    <t>UC03</t>
+  </si>
+  <si>
+    <t>UC04</t>
+  </si>
+  <si>
+    <t>UC05</t>
+  </si>
+  <si>
+    <t>UC06</t>
+  </si>
+  <si>
+    <t>UC07</t>
+  </si>
+  <si>
+    <t>UC08</t>
+  </si>
+  <si>
+    <t>UC09</t>
+  </si>
+  <si>
+    <t>UC10</t>
+  </si>
+  <si>
+    <t>Autenticar Veículo</t>
+  </si>
+  <si>
+    <t>Registrar Saída de Veículo</t>
+  </si>
+  <si>
+    <t>Registrar Entrada de Veículo</t>
+  </si>
+  <si>
+    <t>Registrar Veículo</t>
+  </si>
+  <si>
+    <t>Registrar Funcionário</t>
+  </si>
+  <si>
+    <t>Excluir Veículo</t>
+  </si>
+  <si>
+    <t>Manter Vagas</t>
+  </si>
+  <si>
+    <t>Efetuar Consultas</t>
+  </si>
+  <si>
+    <t>Autenticar Usuário</t>
+  </si>
+  <si>
+    <t>Gerenciar Permissões</t>
+  </si>
+  <si>
+    <t>Cancela Eletrônica</t>
+  </si>
+  <si>
+    <t>Funcionário, Gestor</t>
+  </si>
+  <si>
+    <t>Setor Pessoal</t>
+  </si>
+  <si>
+    <t>Gestor</t>
+  </si>
+  <si>
+    <t>Gestor, Funcionário, Setor Administrativo, Setor Pessoal</t>
+  </si>
+  <si>
+    <t>Funcionário, Gestor, Setor Administrativo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -198,6 +284,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -216,10 +318,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -240,8 +346,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -541,25 +657,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="7.42578125" customWidth="1"/>
+    <col min="1" max="1" width="7.5" customWidth="1"/>
     <col min="2" max="2" width="65" customWidth="1"/>
-    <col min="3" max="3" width="42.140625" customWidth="1"/>
+    <col min="3" max="3" width="35.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="23">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
         <v>13</v>
       </c>
@@ -570,7 +686,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="28">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -581,7 +697,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -592,7 +708,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" s="7" t="s">
         <v>3</v>
       </c>
@@ -604,7 +720,7 @@
       </c>
       <c r="D5" s="6"/>
     </row>
-    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="28">
       <c r="A6" s="7" t="s">
         <v>4</v>
       </c>
@@ -616,7 +732,7 @@
       </c>
       <c r="D6" s="6"/>
     </row>
-    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="28">
       <c r="A7" s="7" t="s">
         <v>5</v>
       </c>
@@ -628,7 +744,7 @@
       </c>
       <c r="D7" s="6"/>
     </row>
-    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="28">
       <c r="A8" s="7" t="s">
         <v>6</v>
       </c>
@@ -640,7 +756,7 @@
       </c>
       <c r="D8" s="6"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="7" t="s">
         <v>7</v>
       </c>
@@ -652,7 +768,7 @@
       </c>
       <c r="D9" s="5"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" s="7" t="s">
         <v>8</v>
       </c>
@@ -664,7 +780,7 @@
       </c>
       <c r="D10" s="5"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="A11" s="7" t="s">
         <v>9</v>
       </c>
@@ -676,7 +792,7 @@
       </c>
       <c r="D11" s="6"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="A12" s="7" t="s">
         <v>10</v>
       </c>
@@ -688,7 +804,7 @@
       </c>
       <c r="D12" s="6"/>
     </row>
-    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="28">
       <c r="A13" s="7" t="s">
         <v>11</v>
       </c>
@@ -700,7 +816,7 @@
       </c>
       <c r="D13" s="6"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="A14" s="7" t="s">
         <v>12</v>
       </c>
@@ -712,7 +828,7 @@
       </c>
       <c r="D14" s="6"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4">
       <c r="A15" s="7" t="s">
         <v>15</v>
       </c>
@@ -724,7 +840,7 @@
       </c>
       <c r="D15" s="6"/>
     </row>
-    <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="28">
       <c r="A16" s="7" t="s">
         <v>16</v>
       </c>
@@ -736,7 +852,7 @@
       </c>
       <c r="D16" s="6"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4">
       <c r="A17" s="7" t="s">
         <v>17</v>
       </c>
@@ -744,7 +860,7 @@
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4">
       <c r="A18" s="7" t="s">
         <v>18</v>
       </c>
@@ -752,7 +868,7 @@
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4">
       <c r="A19" s="7" t="s">
         <v>20</v>
       </c>
@@ -760,7 +876,7 @@
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4">
       <c r="A20" s="7" t="s">
         <v>21</v>
       </c>
@@ -768,7 +884,7 @@
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4">
       <c r="A21" s="7" t="s">
         <v>22</v>
       </c>
@@ -776,7 +892,7 @@
       <c r="C21" s="4"/>
       <c r="D21" s="5"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4">
       <c r="A22" s="7" t="s">
         <v>23</v>
       </c>
@@ -784,7 +900,7 @@
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4">
       <c r="A23" s="7" t="s">
         <v>24</v>
       </c>
@@ -792,7 +908,7 @@
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4">
       <c r="A24" s="7" t="s">
         <v>25</v>
       </c>
@@ -800,16 +916,145 @@
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4">
       <c r="A26" s="7"/>
-      <c r="B26" s="4"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B27" s="4"/>
+      <c r="B26" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C27" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B28" t="s">
+        <v>62</v>
+      </c>
+      <c r="C28" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C29" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C30" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C31" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C32" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B33" t="s">
+        <v>67</v>
+      </c>
+      <c r="C33" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C34" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C35" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C36" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="B37" s="5"/>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="B38" s="6"/>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="B39" s="4"/>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="B40" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -819,9 +1064,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -831,8 +1081,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>